<commit_message>
Revert "nouveau commit excel"
This reverts commit 8ed9f66f549f8b8a4adb00dcaa6359e5e87440db.
</commit_message>
<xml_diff>
--- a/excercise.xlsx
+++ b/excercise.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>sdfd</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>sdssdsf</t>
-  </si>
-  <si>
-    <t>sfsdfsdf4</t>
   </si>
 </sst>
 </file>
@@ -348,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:D11"/>
+  <dimension ref="D1:D6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -371,11 +368,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
push to branch1 5555
</commit_message>
<xml_diff>
--- a/excercise.xlsx
+++ b/excercise.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>sdfd</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>ajouter 0822</t>
+  </si>
+  <si>
+    <t>before merge</t>
   </si>
 </sst>
 </file>
@@ -348,32 +351,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:D8"/>
+  <dimension ref="D1:E11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "push to branch1 5555"
This reverts commit 369a456b2af963b5dba1039121fe4ed3c41f6009.

# Conflicts:
#	excercise.xlsx
</commit_message>
<xml_diff>
--- a/excercise.xlsx
+++ b/excercise.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>sdfd</t>
   </si>
@@ -31,12 +31,6 @@
   </si>
   <si>
     <t>ajouter 0822</t>
-  </si>
-  <si>
-    <t>before merge</t>
-  </si>
-  <si>
-    <t>after</t>
   </si>
 </sst>
 </file>
@@ -354,42 +348,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:E13"/>
+  <dimension ref="D1:D8"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push to branch1 5555" recommited11
</commit_message>
<xml_diff>
--- a/excercise.xlsx
+++ b/excercise.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>sdfd</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>ajouter 0822</t>
+  </si>
+  <si>
+    <t>before merge</t>
+  </si>
+  <si>
+    <t>after</t>
   </si>
 </sst>
 </file>
@@ -348,32 +354,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:D8"/>
+  <dimension ref="D1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>